<commit_message>
Backup QR Scanner data - 2025-11-05T07:33:54.014Z - Cache Bust: 1762328034015
</commit_message>
<xml_diff>
--- a/log_history/Y2_B2526_Anatomy_scanner1762322482932_d32a41f0edf027fbaba50a548472bb628aaf9f0745a69b0f7306d7205f001922.xlsx
+++ b/log_history/Y2_B2526_Anatomy_scanner1762322482932_d32a41f0edf027fbaba50a548472bb628aaf9f0745a69b0f7306d7205f001922.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2022,9 +2022,69 @@
         <v>nahla.nagiub@med.asu.edu.eg</v>
       </c>
     </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>234928</v>
+      </c>
+      <c r="B82" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C82" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D82" t="str">
+        <v>09:07:54</v>
+      </c>
+      <c r="E82" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F82" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>234089</v>
+      </c>
+      <c r="B83" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C83" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D83" t="str">
+        <v>09:17:39</v>
+      </c>
+      <c r="E83" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F83" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>234137</v>
+      </c>
+      <c r="B84" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C84" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D84" t="str">
+        <v>09:19:56</v>
+      </c>
+      <c r="E84" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F84" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F81"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F84"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Backup QR Scanner data - 2025-11-05T18:18:22.034Z - Cache Bust: 1762366702034
</commit_message>
<xml_diff>
--- a/log_history/Y2_B2526_Anatomy_scanner1762322482932_d32a41f0edf027fbaba50a548472bb628aaf9f0745a69b0f7306d7205f001922.xlsx
+++ b/log_history/Y2_B2526_Anatomy_scanner1762322482932_d32a41f0edf027fbaba50a548472bb628aaf9f0745a69b0f7306d7205f001922.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Session" sheetId="1" r:id="rId1"/>
+    <sheet name="Anatomy" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F127"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2082,9 +2082,869 @@
         <v>nahla.nagiub@med.asu.edu.eg</v>
       </c>
     </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>244942</v>
+      </c>
+      <c r="B85" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C85" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D85" t="str">
+        <v>10:08:41</v>
+      </c>
+      <c r="E85" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F85" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>244968</v>
+      </c>
+      <c r="B86" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C86" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D86" t="str">
+        <v>10:08:46</v>
+      </c>
+      <c r="E86" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F86" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>244938</v>
+      </c>
+      <c r="B87" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C87" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D87" t="str">
+        <v>10:08:51</v>
+      </c>
+      <c r="E87" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F87" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>244934</v>
+      </c>
+      <c r="B88" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C88" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D88" t="str">
+        <v>10:08:53</v>
+      </c>
+      <c r="E88" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F88" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>244940</v>
+      </c>
+      <c r="B89" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C89" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D89" t="str">
+        <v>10:08:59</v>
+      </c>
+      <c r="E89" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F89" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>244925</v>
+      </c>
+      <c r="B90" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C90" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D90" t="str">
+        <v>10:09:06</v>
+      </c>
+      <c r="E90" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F90" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>234696</v>
+      </c>
+      <c r="B91" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C91" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D91" t="str">
+        <v>10:09:32</v>
+      </c>
+      <c r="E91" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F91" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>234118</v>
+      </c>
+      <c r="B92" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C92" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D92" t="str">
+        <v>10:09:38</v>
+      </c>
+      <c r="E92" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F92" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>234128</v>
+      </c>
+      <c r="B93" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C93" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D93" t="str">
+        <v>10:09:45</v>
+      </c>
+      <c r="E93" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F93" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>244897</v>
+      </c>
+      <c r="B94" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C94" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D94" t="str">
+        <v>10:10:16</v>
+      </c>
+      <c r="E94" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F94" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>234216</v>
+      </c>
+      <c r="B95" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C95" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D95" t="str">
+        <v>10:10:34</v>
+      </c>
+      <c r="E95" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F95" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>234094</v>
+      </c>
+      <c r="B96" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C96" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D96" t="str">
+        <v>10:10:45</v>
+      </c>
+      <c r="E96" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F96" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>234215</v>
+      </c>
+      <c r="B97" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C97" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D97" t="str">
+        <v>10:10:57</v>
+      </c>
+      <c r="E97" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F97" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>234171</v>
+      </c>
+      <c r="B98" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C98" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D98" t="str">
+        <v>10:11:03</v>
+      </c>
+      <c r="E98" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F98" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>244956</v>
+      </c>
+      <c r="B99" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C99" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D99" t="str">
+        <v>10:11:07</v>
+      </c>
+      <c r="E99" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F99" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>244941</v>
+      </c>
+      <c r="B100" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C100" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D100" t="str">
+        <v>10:11:08</v>
+      </c>
+      <c r="E100" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F100" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>244949</v>
+      </c>
+      <c r="B101" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C101" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D101" t="str">
+        <v>10:11:45</v>
+      </c>
+      <c r="E101" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F101" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>234347</v>
+      </c>
+      <c r="B102" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C102" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D102" t="str">
+        <v>10:11:51</v>
+      </c>
+      <c r="E102" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F102" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>234336</v>
+      </c>
+      <c r="B103" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C103" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D103" t="str">
+        <v>10:11:56</v>
+      </c>
+      <c r="E103" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F103" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v>234191</v>
+      </c>
+      <c r="B104" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C104" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D104" t="str">
+        <v>10:12:27</v>
+      </c>
+      <c r="E104" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F104" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v>234193</v>
+      </c>
+      <c r="B105" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C105" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D105" t="str">
+        <v>10:12:40</v>
+      </c>
+      <c r="E105" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F105" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v>234116</v>
+      </c>
+      <c r="B106" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C106" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D106" t="str">
+        <v>10:12:46</v>
+      </c>
+      <c r="E106" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F106" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>234219</v>
+      </c>
+      <c r="B107" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C107" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D107" t="str">
+        <v>10:12:54</v>
+      </c>
+      <c r="E107" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F107" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>244902</v>
+      </c>
+      <c r="B108" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C108" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D108" t="str">
+        <v>10:13:08</v>
+      </c>
+      <c r="E108" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F108" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>234241</v>
+      </c>
+      <c r="B109" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C109" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D109" t="str">
+        <v>10:13:24</v>
+      </c>
+      <c r="E109" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F109" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v>234098</v>
+      </c>
+      <c r="B110" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C110" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D110" t="str">
+        <v>10:13:48</v>
+      </c>
+      <c r="E110" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F110" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>244896</v>
+      </c>
+      <c r="B111" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C111" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D111" t="str">
+        <v>10:20:04</v>
+      </c>
+      <c r="E111" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F111" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>244736</v>
+      </c>
+      <c r="B112" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C112" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D112" t="str">
+        <v>10:20:11</v>
+      </c>
+      <c r="E112" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F112" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v>244672</v>
+      </c>
+      <c r="B113" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C113" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D113" t="str">
+        <v>10:20:32</v>
+      </c>
+      <c r="E113" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F113" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v>244841</v>
+      </c>
+      <c r="B114" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C114" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D114" t="str">
+        <v>10:22:34</v>
+      </c>
+      <c r="E114" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F114" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>244656</v>
+      </c>
+      <c r="B115" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C115" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D115" t="str">
+        <v>10:22:59</v>
+      </c>
+      <c r="E115" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F115" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <v>244785</v>
+      </c>
+      <c r="B116" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C116" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D116" t="str">
+        <v>10:24:32</v>
+      </c>
+      <c r="E116" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F116" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <v>244756</v>
+      </c>
+      <c r="B117" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C117" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D117" t="str">
+        <v>10:24:47</v>
+      </c>
+      <c r="E117" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F117" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <v>244647</v>
+      </c>
+      <c r="B118" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C118" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D118" t="str">
+        <v>10:26:58</v>
+      </c>
+      <c r="E118" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F118" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <v>244645</v>
+      </c>
+      <c r="B119" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C119" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D119" t="str">
+        <v>10:27:10</v>
+      </c>
+      <c r="E119" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F119" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>244893</v>
+      </c>
+      <c r="B120" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C120" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D120" t="str">
+        <v>10:28:17</v>
+      </c>
+      <c r="E120" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F120" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>244937</v>
+      </c>
+      <c r="B121" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C121" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D121" t="str">
+        <v>10:28:24</v>
+      </c>
+      <c r="E121" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F121" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="str">
+        <v>244714</v>
+      </c>
+      <c r="B122" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C122" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D122" t="str">
+        <v>10:28:33</v>
+      </c>
+      <c r="E122" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F122" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="str">
+        <v>244765</v>
+      </c>
+      <c r="B123" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C123" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D123" t="str">
+        <v>10:32:09</v>
+      </c>
+      <c r="E123" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F123" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="str">
+        <v>244906</v>
+      </c>
+      <c r="B124" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C124" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D124" t="str">
+        <v>10:32:46</v>
+      </c>
+      <c r="E124" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F124" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="str">
+        <v>234829</v>
+      </c>
+      <c r="B125" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C125" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D125" t="str">
+        <v>10:38:34</v>
+      </c>
+      <c r="E125" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F125" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="str">
+        <v>234823</v>
+      </c>
+      <c r="B126" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C126" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D126" t="str">
+        <v>10:38:57</v>
+      </c>
+      <c r="E126" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F126" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="str">
+        <v>234830</v>
+      </c>
+      <c r="B127" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C127" t="str">
+        <v>05/11/2025</v>
+      </c>
+      <c r="D127" t="str">
+        <v>10:39:16</v>
+      </c>
+      <c r="E127" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F127" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F84"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F127"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>